<commit_message>
ppt sidang need revision proposal done, but need revision like ppt revisi proposal dari dosbing initiated.
</commit_message>
<xml_diff>
--- a/manual_extraction_feature.xlsx
+++ b/manual_extraction_feature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\5112100100\S2\Bismillah Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BC7596-F7CA-477D-951C-3778A658844B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="SKPL-1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="SKPL-3" sheetId="5" r:id="rId3"/>
     <sheet name="SKPL-4" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3000,8 +3001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD37E1F5-3BB0-4196-9B95-AD169E9BC188}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,8 +4920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27993049-2CCD-4834-B543-67CBD9F6FBE5}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
checkpoint sebelum buku, program alur utama selesai. untuk selanjutnya setiap ada perubahan harus commit.
</commit_message>
<xml_diff>
--- a/manual_extraction_feature.xlsx
+++ b/manual_extraction_feature.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\5112100100\S2\Bismillah Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BC7596-F7CA-477D-951C-3778A658844B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D71E8-039F-4063-94DB-ED9C1F381AAD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="SKPL-1" sheetId="1" r:id="rId1"/>
-    <sheet name="SKPL-2" sheetId="3" r:id="rId2"/>
-    <sheet name="SKPL-3" sheetId="5" r:id="rId3"/>
-    <sheet name="SKPL-4" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="SKPL-2" sheetId="3" r:id="rId3"/>
+    <sheet name="SKPL-3" sheetId="5" r:id="rId4"/>
+    <sheet name="SKPL-4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="134">
   <si>
     <t>Requirement</t>
   </si>
@@ -337,6 +343,99 @@
   </si>
   <si>
     <t>df</t>
+  </si>
+  <si>
+    <t>dok_1</t>
+  </si>
+  <si>
+    <t>dok_2</t>
+  </si>
+  <si>
+    <t>dok_3</t>
+  </si>
+  <si>
+    <t>dok_4</t>
+  </si>
+  <si>
+    <t>view information of requested tutorial</t>
+  </si>
+  <si>
+    <t>view information of accepted tutorial</t>
+  </si>
+  <si>
+    <t>respond requested tutorial</t>
+  </si>
+  <si>
+    <t>cancel responded tutorial</t>
+  </si>
+  <si>
+    <t>show information of lecturer's presence</t>
+  </si>
+  <si>
+    <t>search for lecturer</t>
+  </si>
+  <si>
+    <t>register new account</t>
+  </si>
+  <si>
+    <t>show and edit lecturer's biodata</t>
+  </si>
+  <si>
+    <t>edit student's biodata</t>
+  </si>
+  <si>
+    <t>register new lecturer's account</t>
+  </si>
+  <si>
+    <t>delete lecturer's account</t>
+  </si>
+  <si>
+    <t>update lecturer's account information</t>
+  </si>
+  <si>
+    <t>add lecturer's availability status</t>
+  </si>
+  <si>
+    <t>update lecturer's availability status</t>
+  </si>
+  <si>
+    <t>delete lecturer's availability status</t>
+  </si>
+  <si>
+    <t>show lecturer's information and availability status</t>
+  </si>
+  <si>
+    <t>search for lecturer's account</t>
+  </si>
+  <si>
+    <t>lecturer can approve student's plan</t>
+  </si>
+  <si>
+    <t>register new user account</t>
+  </si>
+  <si>
+    <t>edit user profile</t>
+  </si>
+  <si>
+    <t>report find lost items</t>
+  </si>
+  <si>
+    <t>report loss of item</t>
+  </si>
+  <si>
+    <t>asking help in term of question</t>
+  </si>
+  <si>
+    <t>delete user account</t>
+  </si>
+  <si>
+    <t>give an award</t>
+  </si>
+  <si>
+    <t>make a request of tutorial</t>
+  </si>
+  <si>
+    <t>make addition to participant of a tutorial</t>
   </si>
 </sst>
 </file>
@@ -705,7 +804,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +817,7 @@
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1661,16 +1760,15 @@
         <v>0.13463726805734305</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" ref="K21:M26" si="11">AVERAGE(F21:J21)</f>
-        <v>8.6805495655449219E-2</v>
+        <f>_xlfn.STDEV.S(E21:I21)</f>
+        <v>0.15321947174801229</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="11"/>
-        <v>7.4227573764548749E-2</v>
+        <f>MAX(E21:I21)</f>
+        <v>0.37379613006681212</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="11"/>
-        <v>8.9073088517458501E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1700,20 +1798,19 @@
         <v>0.19471733430875102</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" ref="J22:J26" si="12">AVERAGE(E22:I22)</f>
+        <f t="shared" ref="J22:J26" si="11">AVERAGE(E22:I22)</f>
         <v>0.11370269287511263</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="11"/>
-        <v>6.1684005436772729E-2</v>
+        <f t="shared" ref="K22:K26" si="12">_xlfn.STDEV.S(E22:I22)</f>
+        <v>0.16807503926666958</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="11"/>
-        <v>7.4020806524127264E-2</v>
+        <f t="shared" ref="L22:L26" si="13">MAX(E22:I22)</f>
+        <v>0.37379613006681212</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="11"/>
-        <v>8.8824967828952731E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1743,20 +1840,19 @@
         <v>0</v>
       </c>
       <c r="J23" s="2">
+        <f t="shared" si="11"/>
+        <v>0.13646345212677896</v>
+      </c>
+      <c r="K23" s="2">
         <f t="shared" si="12"/>
-        <v>0.13646345212677896</v>
-      </c>
-      <c r="K23" s="2">
-        <f t="shared" si="11"/>
-        <v>0.13381712153014441</v>
+        <v>0.13399524976542304</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="11"/>
-        <v>0.16058054583617332</v>
+        <f t="shared" si="13"/>
+        <v>0.28472943679875407</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="11"/>
-        <v>0.14311811125837015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1786,20 +1882,19 @@
         <v>0</v>
       </c>
       <c r="J24" s="2">
+        <f t="shared" si="11"/>
+        <v>4.957854374503784E-2</v>
+      </c>
+      <c r="K24" s="2">
         <f t="shared" si="12"/>
-        <v>4.957854374503784E-2</v>
-      </c>
-      <c r="K24" s="2">
-        <f t="shared" si="11"/>
-        <v>5.9494252494045406E-2</v>
+        <v>0.11086099403935161</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="11"/>
-        <v>7.1393102992854479E-2</v>
+        <f t="shared" si="13"/>
+        <v>0.2478927187251892</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="11"/>
-        <v>3.6093179846387546E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1825,20 +1920,19 @@
         <v>0.39178282449176549</v>
       </c>
       <c r="J25" s="2">
+        <f t="shared" si="11"/>
+        <v>0.16524147328009423</v>
+      </c>
+      <c r="K25" s="2">
         <f t="shared" si="12"/>
-        <v>0.16524147328009423</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="11"/>
-        <v>0.16835074691412275</v>
+        <v>0.17352920199600425</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="11"/>
-        <v>0.20202089629694728</v>
+        <f t="shared" si="13"/>
+        <v>0.39178282449176549</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="11"/>
-        <v>0.18547918819658596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1868,20 +1962,19 @@
         <v>0.39178282449176549</v>
       </c>
       <c r="J26" s="2">
+        <f t="shared" si="11"/>
+        <v>0.11730003176010331</v>
+      </c>
+      <c r="K26" s="2">
         <f t="shared" si="12"/>
-        <v>0.11730003176010331</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="11"/>
-        <v>0.14076003811212395</v>
+        <v>0.17508007781615617</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="11"/>
-        <v>0.12996857887279853</v>
+        <f t="shared" si="13"/>
+        <v>0.39178282449176549</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="11"/>
-        <v>0.15596229464735825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1889,7 +1982,7 @@
         <v>21</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:B29" si="13">(SUMPRODUCT($B$13:$O$13,B15:O15)/($P$13*P15))</f>
+        <f t="shared" ref="B27:B29" si="14">(SUMPRODUCT($B$13:$O$13,B15:O15)/($P$13*P15))</f>
         <v>0</v>
       </c>
     </row>
@@ -1898,7 +1991,7 @@
         <v>22</v>
       </c>
       <c r="B28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -1907,7 +2000,7 @@
         <v>43</v>
       </c>
       <c r="B29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.19471733430875102</v>
       </c>
     </row>
@@ -1930,7 +2023,7 @@
         <v>22</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:B33" si="14">(SUMPRODUCT($B$14:$O$14,B16:O16)/($P$14*P16))</f>
+        <f t="shared" ref="B32:B33" si="15">(SUMPRODUCT($B$14:$O$14,B16:O16)/($P$14*P16))</f>
         <v>0.28472943679875407</v>
       </c>
     </row>
@@ -1939,7 +2032,7 @@
         <v>43</v>
       </c>
       <c r="B33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1986,11 +2079,408 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28894055-7F27-471F-8199-8B27A85BFA58}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08811567-DF03-4C57-93EC-C0FA72CC352F}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,12 +3487,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD37E1F5-3BB0-4196-9B95-AD169E9BC188}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4916,12 +5406,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27993049-2CCD-4834-B543-67CBD9F6FBE5}">
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
merapikan dokumen perhitungan manual
</commit_message>
<xml_diff>
--- a/manual_extraction_feature.xlsx
+++ b/manual_extraction_feature.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\5112100100\S2\Bismillah Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bismillahtesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D71E8-039F-4063-94DB-ED9C1F381AAD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B12F41B-86D6-42BF-9818-E8741BB74343}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F5712EEC-BBCF-4C01-98FD-C3C7C79CD6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="SKPL-1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="SKPL-2" sheetId="3" r:id="rId3"/>
-    <sheet name="SKPL-3" sheetId="5" r:id="rId4"/>
-    <sheet name="SKPL-4" sheetId="6" r:id="rId5"/>
+    <sheet name="SKPL-2" sheetId="3" r:id="rId2"/>
+    <sheet name="SKPL-3" sheetId="5" r:id="rId3"/>
+    <sheet name="SKPL-4" sheetId="6" r:id="rId4"/>
+    <sheet name="Label" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="136">
   <si>
     <t>Requirement</t>
   </si>
@@ -120,9 +121,6 @@
     <t>sim d4</t>
   </si>
   <si>
-    <t>fitur</t>
-  </si>
-  <si>
     <t>rerata</t>
   </si>
   <si>
@@ -436,6 +434,15 @@
   </si>
   <si>
     <t>make addition to participant of a tutorial</t>
+  </si>
+  <si>
+    <t>Fitur</t>
+  </si>
+  <si>
+    <t>Vektor similarity masing masing dokumen(requirement)</t>
+  </si>
+  <si>
+    <t>Vektor similaritas masing-masing dokumen(requirement)</t>
   </si>
 </sst>
 </file>
@@ -801,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2EF124-D346-452A-982B-FDB79086BD2F}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,40 +842,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
         <v>13</v>
       </c>
       <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
       </c>
       <c r="P1" t="s">
         <v>17</v>
@@ -876,7 +883,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -927,7 +934,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -978,7 +985,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1029,7 +1036,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1080,7 +1087,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1131,7 +1138,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1307,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="P11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1637,7 +1644,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <f t="shared" ref="B17:O17" si="9">(B7/$P7)*B$9</f>
@@ -1702,7 +1709,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1713,21 +1720,6 @@
         <f>(SUMPRODUCT($B$12:$O$12,B13:O13)/($P$12*P13))</f>
         <v>0.37379613006681212</v>
       </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M20" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1737,39 +1729,6 @@
         <f t="shared" ref="B21:B23" si="10">(SUMPRODUCT($B$12:$O$12,B14:O14)/($P$12*P14))</f>
         <v>0.14969510510995152</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21">
-        <v>0.37379613006681212</v>
-      </c>
-      <c r="F21">
-        <v>0.14969510510995152</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0.14969510510995152</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <f>AVERAGE(E21:I21)</f>
-        <v>0.13463726805734305</v>
-      </c>
-      <c r="K21" s="2">
-        <f>_xlfn.STDEV.S(E21:I21)</f>
-        <v>0.15321947174801229</v>
-      </c>
-      <c r="L21" s="2">
-        <f>MAX(E21:I21)</f>
-        <v>0.37379613006681212</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1779,39 +1738,6 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22">
-        <v>0.37379613006681212</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0.19471733430875102</v>
-      </c>
-      <c r="J22" s="2">
-        <f t="shared" ref="J22:J26" si="11">AVERAGE(E22:I22)</f>
-        <v>0.11370269287511263</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" ref="K22:K26" si="12">_xlfn.STDEV.S(E22:I22)</f>
-        <v>0.16807503926666958</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" ref="L22:L26" si="13">MAX(E22:I22)</f>
-        <v>0.37379613006681212</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1821,118 +1747,19 @@
         <f t="shared" si="10"/>
         <v>0.14969510510995152</v>
       </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23">
-        <v>0.14969510510995152</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0.2478927187251892</v>
-      </c>
-      <c r="H23">
-        <v>0.28472943679875407</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <f t="shared" si="11"/>
-        <v>0.13646345212677896</v>
-      </c>
-      <c r="K23" s="2">
-        <f t="shared" si="12"/>
-        <v>0.13399524976542304</v>
-      </c>
-      <c r="L23" s="2">
-        <f t="shared" si="13"/>
-        <v>0.28472943679875407</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <f>(SUMPRODUCT($B$12:$O$12,B17:O17)/($P$12*P17))</f>
         <v>0</v>
       </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0.2478927187251892</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <f t="shared" si="11"/>
-        <v>4.957854374503784E-2</v>
-      </c>
-      <c r="K24" s="2">
-        <f t="shared" si="12"/>
-        <v>0.11086099403935161</v>
-      </c>
-      <c r="L24" s="2">
-        <f t="shared" si="13"/>
-        <v>0.2478927187251892</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25">
-        <v>0.14969510510995152</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0.28472943679875407</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0.39178282449176549</v>
-      </c>
-      <c r="J25" s="2">
-        <f t="shared" si="11"/>
-        <v>0.16524147328009423</v>
-      </c>
-      <c r="K25" s="2">
-        <f t="shared" si="12"/>
-        <v>0.17352920199600425</v>
-      </c>
-      <c r="L25" s="2">
-        <f t="shared" si="13"/>
-        <v>0.39178282449176549</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1943,46 +1770,13 @@
         <f>(SUMPRODUCT($B$13:$O$13,B14:O14)/($P$13*P14))</f>
         <v>0</v>
       </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0.19471733430875102</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0.39178282449176549</v>
-      </c>
-      <c r="J26" s="2">
-        <f t="shared" si="11"/>
-        <v>0.11730003176010331</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="12"/>
-        <v>0.17508007781615617</v>
-      </c>
-      <c r="L26" s="2">
-        <f t="shared" si="13"/>
-        <v>0.39178282449176549</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:B29" si="14">(SUMPRODUCT($B$13:$O$13,B15:O15)/($P$13*P15))</f>
+        <f t="shared" ref="B27:B29" si="11">(SUMPRODUCT($B$13:$O$13,B15:O15)/($P$13*P15))</f>
         <v>0</v>
       </c>
     </row>
@@ -1991,22 +1785,22 @@
         <v>22</v>
       </c>
       <c r="B28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.19471733430875102</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2023,25 +1817,25 @@
         <v>22</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:B33" si="15">(SUMPRODUCT($B$14:$O$14,B16:O16)/($P$14*P16))</f>
+        <f t="shared" ref="B32:B33" si="12">(SUMPRODUCT($B$14:$O$14,B16:O16)/($P$14*P16))</f>
         <v>0.28472943679875407</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2050,27 +1844,289 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <f>(SUMPRODUCT($B$15:$O$15,B17:O17)/($P$15*P17))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <f>(SUMPRODUCT($B$16:$O$16,B17:O17)/($P$16*P17))</f>
         <v>0.39178282449176549</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>0.37379613006681212</v>
+      </c>
+      <c r="C41">
+        <v>0.14969510510995152</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0.14969510510995152</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>0.37379613006681212</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0.19471733430875102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>0.14969510510995152</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.2478927187251892</v>
+      </c>
+      <c r="E43">
+        <v>0.28472943679875407</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.2478927187251892</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <v>0.14969510510995152</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.28472943679875407</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0.39178282449176549</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0.19471733430875102</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0.39178282449176549</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="2">
+        <f>AVERAGE(B41:F41)</f>
+        <v>0.13463726805734305</v>
+      </c>
+      <c r="C49" s="2">
+        <f>_xlfn.STDEV.S(B41:F41)</f>
+        <v>0.15321947174801229</v>
+      </c>
+      <c r="D49" s="2">
+        <f>MAX(B41:F41)</f>
+        <v>0.37379613006681212</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="2">
+        <f>AVERAGE(B42:F42)</f>
+        <v>0.11370269287511263</v>
+      </c>
+      <c r="C50" s="2">
+        <f>_xlfn.STDEV.S(B42:F42)</f>
+        <v>0.16807503926666958</v>
+      </c>
+      <c r="D50" s="2">
+        <f>MAX(B42:F42)</f>
+        <v>0.37379613006681212</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="2">
+        <f>AVERAGE(B43:F43)</f>
+        <v>0.13646345212677896</v>
+      </c>
+      <c r="C51" s="2">
+        <f>_xlfn.STDEV.S(B43:F43)</f>
+        <v>0.13399524976542304</v>
+      </c>
+      <c r="D51" s="2">
+        <f>MAX(B43:F43)</f>
+        <v>0.28472943679875407</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="2">
+        <f>AVERAGE(B44:F44)</f>
+        <v>4.957854374503784E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <f>_xlfn.STDEV.S(B44:F44)</f>
+        <v>0.11086099403935161</v>
+      </c>
+      <c r="D52" s="2">
+        <f>MAX(B44:F44)</f>
+        <v>0.2478927187251892</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="2">
+        <f>AVERAGE(B45:F45)</f>
+        <v>0.16524147328009423</v>
+      </c>
+      <c r="C53" s="2">
+        <f>_xlfn.STDEV.S(B45:F45)</f>
+        <v>0.17352920199600425</v>
+      </c>
+      <c r="D53" s="2">
+        <f>MAX(B45:F45)</f>
+        <v>0.39178282449176549</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="2">
+        <f>AVERAGE(B46:F46)</f>
+        <v>0.11730003176010331</v>
+      </c>
+      <c r="C54" s="2">
+        <f>_xlfn.STDEV.S(B46:F46)</f>
+        <v>0.17508007781615617</v>
+      </c>
+      <c r="D54" s="2">
+        <f>MAX(B46:F46)</f>
+        <v>0.39178282449176549</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2079,408 +2135,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28894055-7F27-471F-8199-8B27A85BFA58}">
-  <dimension ref="A1:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08811567-DF03-4C57-93EC-C0FA72CC352F}">
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08811567-DF03-4C57-93EC-C0FA72CC352F}">
-  <dimension ref="A1:O37"/>
-  <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,7 +2207,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2596,7 +2255,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2644,7 +2303,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2692,7 +2351,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2740,7 +2399,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3213,12 +2872,12 @@
         <v>0.29912308279838712</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3227,7 +2886,7 @@
         <v>4.4634102837990915E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3236,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -3245,7 +2904,7 @@
         <v>0.26338106285442126</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3254,12 +2913,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3268,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3277,7 +2936,7 @@
         <v>6.7094269341510845E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3286,12 +2945,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3300,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -3309,12 +2968,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3323,21 +2982,12 @@
         <v>0.48742752518600441</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -3353,132 +3003,171 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="2">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>4.4634102837990915E-2</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>6.7094269341510845E-2</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>0.26338106285442126</v>
+      </c>
+      <c r="C36">
+        <v>6.7094269341510845E-2</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0.48742752518600441</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0.48742752518600441</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="2">
         <f>AVERAGE(B33:E33)</f>
         <v>7.7003791423103041E-2</v>
       </c>
-      <c r="G33" s="2">
+      <c r="C41" s="2">
         <f>_xlfn.STDEV.S(B33:E33)</f>
         <v>0.12602043727420553</v>
       </c>
-      <c r="H33" s="2">
+      <c r="D41" s="2">
         <f>MAX(B33:E33)</f>
         <v>0.26338106285442126</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>19</v>
       </c>
-      <c r="B34">
-        <v>4.4634102837990915E-2</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="B42" s="2">
+        <f>AVERAGE(B34:E34)</f>
+        <v>2.7932093044875442E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <f>_xlfn.STDEV.S(B34:E34)</f>
+        <v>3.3531263159193365E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <f>MAX(B34:E34)</f>
         <v>6.7094269341510845E-2</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" ref="F34:F37" si="11">AVERAGE(B34:E34)</f>
-        <v>2.7932093044875442E-2</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" ref="G34:G37" si="12">_xlfn.STDEV.S(B34:E34)</f>
-        <v>3.3531263159193365E-2</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" ref="H34:H37" si="13">MAX(B34:E34)</f>
-        <v>6.7094269341510845E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>20</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B43" s="2">
+        <f>AVERAGE(B35:E35)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <f>_xlfn.STDEV.S(B35:E35)</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <f>MAX(B35:E35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>21</v>
       </c>
-      <c r="B36">
-        <v>0.26338106285442126</v>
-      </c>
-      <c r="C36">
-        <v>6.7094269341510845E-2</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
+      <c r="B44" s="2">
+        <f>AVERAGE(B36:E36)</f>
+        <v>0.20447571434548412</v>
+      </c>
+      <c r="C44" s="2">
+        <f>_xlfn.STDEV.S(B36:E36)</f>
+        <v>0.21925293348806435</v>
+      </c>
+      <c r="D44" s="2">
+        <f>MAX(B36:E36)</f>
         <v>0.48742752518600441</v>
       </c>
-      <c r="F36" s="2">
-        <f t="shared" si="11"/>
-        <v>0.20447571434548412</v>
-      </c>
-      <c r="G36" s="2">
-        <f t="shared" si="12"/>
-        <v>0.21925293348806435</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="13"/>
-        <v>0.48742752518600441</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>22</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0.48742752518600441</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="11"/>
+      <c r="B45" s="2">
+        <f>AVERAGE(B37:E37)</f>
         <v>0.1218568812965011</v>
       </c>
-      <c r="G37" s="2">
-        <f t="shared" si="12"/>
+      <c r="C45" s="2">
+        <f>_xlfn.STDEV.S(B37:E37)</f>
         <v>0.2437137625930022</v>
       </c>
-      <c r="H37" s="2">
-        <f t="shared" si="13"/>
+      <c r="D45" s="2">
+        <f>MAX(B37:E37)</f>
         <v>0.48742752518600441</v>
       </c>
     </row>
@@ -3487,12 +3176,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD37E1F5-3BB0-4196-9B95-AD169E9BC188}">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3524,7 +3213,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -3533,7 +3222,7 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -3542,16 +3231,16 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
-      </c>
-      <c r="L1" t="s">
-        <v>60</v>
       </c>
       <c r="M1" t="s">
         <v>1</v>
@@ -3563,10 +3252,10 @@
         <v>5</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>62</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
       </c>
       <c r="R1" t="s">
         <v>13</v>
@@ -3577,7 +3266,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3598,7 +3287,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3616,7 +3305,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3637,7 +3326,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3658,7 +3347,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3679,7 +3368,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3700,7 +3389,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3724,7 +3413,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3742,7 +3431,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3763,7 +3452,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <f>COUNTIF(B2:B10,"&gt;0")</f>
@@ -3909,7 +3598,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S14" t="s">
         <v>23</v>
@@ -4302,7 +3991,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <f t="shared" ref="B20:R20" si="9">(B7/$S7)*B$12</f>
@@ -4379,7 +4068,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <f t="shared" ref="B21:R21" si="10">(B8/$S8)*B$12</f>
@@ -4456,7 +4145,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22">
         <f t="shared" ref="B22:R22" si="11">(B9/$S9)*B$12</f>
@@ -4533,7 +4222,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <f t="shared" ref="B23:R23" si="12">(B10/$S10)*B$12</f>
@@ -4610,7 +4299,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -4663,7 +4352,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <f t="shared" si="13"/>
@@ -4675,7 +4364,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31">
         <f t="shared" si="13"/>
@@ -4687,7 +4376,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32">
         <f t="shared" si="13"/>
@@ -4697,21 +4386,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -4720,7 +4409,7 @@
         <v>0.11983660389070357</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -4728,23 +4417,8 @@
         <f t="shared" ref="B36:B41" si="14">(SUMPRODUCT($B$16:$R$16,B18:R18)/($S$16*S18))</f>
         <v>0</v>
       </c>
-      <c r="E36" t="s">
-        <v>28</v>
-      </c>
-      <c r="N36" t="s">
-        <v>29</v>
-      </c>
-      <c r="O36" t="s">
-        <v>30</v>
-      </c>
-      <c r="P36" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -4752,301 +4426,49 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37">
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="G37">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>8.7431103672622051E-2</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37" s="2">
-        <f>AVERAGE(F37:M37)</f>
-        <v>4.9394200292716822E-2</v>
-      </c>
-      <c r="O37" s="2">
-        <f>_xlfn.STDEV.S(F37:M37)</f>
-        <v>7.4764027292336721E-2</v>
-      </c>
-      <c r="P37" s="2">
-        <f>MAX(F37:M37)</f>
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <f>(SUMPRODUCT($B$16:$R$16,B20:R20)/($S$16*S20))</f>
         <v>0.69995793711042931</v>
       </c>
-      <c r="E38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38">
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="G38">
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0.64215249846663691</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0.16431677645163634</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" ref="N38:N45" si="15">AVERAGE(F38:M38)</f>
-        <v>0.1499615062542845</v>
-      </c>
-      <c r="O38" s="2">
-        <f t="shared" ref="O38:O45" si="16">_xlfn.STDEV.S(F38:M38)</f>
-        <v>0.219338057045979</v>
-      </c>
-      <c r="P38" s="2">
-        <f t="shared" ref="P38:P45" si="17">MAX(F38:M38)</f>
-        <v>0.64215249846663691</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="G39">
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>8.7431103672622051E-2</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39" s="2">
-        <f t="shared" si="15"/>
-        <v>4.9394200292716822E-2</v>
-      </c>
-      <c r="O39" s="2">
-        <f t="shared" si="16"/>
-        <v>7.4764027292336721E-2</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="17"/>
-        <v>0.19661138755800142</v>
-      </c>
-      <c r="Q39" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40">
         <f t="shared" si="14"/>
         <v>0.16431677645163634</v>
       </c>
-      <c r="E40" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0.21409949120674793</v>
-      </c>
-      <c r="J40">
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="K40">
-        <v>0.16020903507989245</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" si="15"/>
-        <v>8.1857991034877051E-2</v>
-      </c>
-      <c r="O40" s="2">
-        <f t="shared" si="16"/>
-        <v>0.11748009866307094</v>
-      </c>
-      <c r="P40" s="2">
-        <f t="shared" si="17"/>
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0.21409949120674793</v>
-      </c>
-      <c r="J41">
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="K41">
-        <v>0.16020903507989245</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41" s="2">
-        <f t="shared" si="15"/>
-        <v>8.1857991034877051E-2</v>
-      </c>
-      <c r="O41" s="2">
-        <f t="shared" si="16"/>
-        <v>0.11748009866307094</v>
-      </c>
-      <c r="P41" s="2">
-        <f t="shared" si="17"/>
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="Q41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" t="s">
-        <v>43</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0.64215249846663691</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="J42">
-        <v>0.28055540199237605</v>
-      </c>
-      <c r="K42">
-        <v>0.20993749208047283</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42" s="2">
-        <f t="shared" si="15"/>
-        <v>0.17665009931648273</v>
-      </c>
-      <c r="O42" s="2">
-        <f t="shared" si="16"/>
-        <v>0.22810216643738657</v>
-      </c>
-      <c r="P42" s="2">
-        <f t="shared" si="17"/>
-        <v>0.64215249846663691</v>
-      </c>
-      <c r="Q42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -5054,175 +4476,49 @@
         <f>(SUMPRODUCT($B$17:$R$17,B18:R18)/($S$17*S18))</f>
         <v>0</v>
       </c>
-      <c r="E43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0.16020903507989245</v>
-      </c>
-      <c r="J43">
-        <v>0.16020903507989245</v>
-      </c>
-      <c r="K43">
-        <v>0.20993749208047283</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43" s="2">
-        <f t="shared" si="15"/>
-        <v>6.6294445280032213E-2</v>
-      </c>
-      <c r="O43" s="2">
-        <f t="shared" si="16"/>
-        <v>9.2773143145448794E-2</v>
-      </c>
-      <c r="P43" s="2">
-        <f t="shared" si="17"/>
-        <v>0.20993749208047283</v>
-      </c>
-      <c r="Q43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
       <c r="B44">
-        <f t="shared" ref="B44:B48" si="18">(SUMPRODUCT($B$17:$R$17,B19:R19)/($S$17*S19))</f>
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
+        <f t="shared" ref="B44:B48" si="15">(SUMPRODUCT($B$17:$R$17,B19:R19)/($S$17*S19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="15"/>
+        <v>8.7431103672622051E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>67</v>
       </c>
-      <c r="F44">
-        <v>8.7431103672622051E-2</v>
-      </c>
-      <c r="G44">
-        <v>0.16431677645163634</v>
-      </c>
-      <c r="H44">
-        <v>8.7431103672622051E-2</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44" s="2">
+      <c r="B48">
         <f t="shared" si="15"/>
-        <v>4.2397372974610062E-2</v>
-      </c>
-      <c r="O44" s="2">
-        <f t="shared" si="16"/>
-        <v>6.3141678471170845E-2</v>
-      </c>
-      <c r="P44" s="2">
-        <f t="shared" si="17"/>
-        <v>0.16431677645163634</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45" s="2">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O45" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P45" s="2">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="18"/>
-        <v>8.7431103672622051E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -5245,10 +4541,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51:B54" si="19">(SUMPRODUCT($B$18:$R$18,B20:R20)/($S$18*S20))</f>
+        <f t="shared" ref="B51:B54" si="16">(SUMPRODUCT($B$18:$R$18,B20:R20)/($S$18*S20))</f>
         <v>0.28055540199237605</v>
       </c>
       <c r="F51">
@@ -5257,10 +4553,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>0.16020903507989245</v>
       </c>
       <c r="F52">
@@ -5269,10 +4565,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F53">
@@ -5281,10 +4577,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F54">
@@ -5293,12 +4589,12 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B56">
         <f>(SUMPRODUCT($B$19:$R$19,B20:R20)/($S$19*S20))</f>
@@ -5307,39 +4603,39 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B59" si="20">(SUMPRODUCT($B$19:$R$19,B21:R21)/($S$19*S21))</f>
+        <f t="shared" ref="B57:B59" si="17">(SUMPRODUCT($B$19:$R$19,B21:R21)/($S$19*S21))</f>
         <v>0.16020903507989245</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B58">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <f>(SUMPRODUCT($B$20:$R$20,B21:R21)/($S$20*S21))</f>
@@ -5348,57 +4644,520 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62">
-        <f t="shared" ref="B62:B63" si="21">(SUMPRODUCT($B$20:$R$20,B22:R22)/($S$20*S22))</f>
+        <f t="shared" ref="B62:B63" si="18">(SUMPRODUCT($B$20:$R$20,B22:R22)/($S$20*S22))</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <f>(SUMPRODUCT($B$21:$R$21,B22:R22)/($S$21*S22))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <f>(SUMPRODUCT($B$21:$R$21,B23:R23)/($S$21*S23))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68">
         <f>(SUMPRODUCT($B$22:$R$22,B23:R23)/($S$22*S23))</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71">
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="C71">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>8.7431103672622051E-2</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72">
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="C72">
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0.64215249846663691</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0.16431677645163634</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C73">
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>8.7431103672622051E-2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0.21409949120674793</v>
+      </c>
+      <c r="F74">
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="G74">
+        <v>0.16020903507989245</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0.21409949120674793</v>
+      </c>
+      <c r="F75">
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="G75">
+        <v>0.16020903507989245</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0.64215249846663691</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="F76">
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="G76">
+        <v>0.20993749208047283</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0.16020903507989245</v>
+      </c>
+      <c r="F77">
+        <v>0.16020903507989245</v>
+      </c>
+      <c r="G77">
+        <v>0.20993749208047283</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78">
+        <v>8.7431103672622051E-2</v>
+      </c>
+      <c r="C78">
+        <v>0.16431677645163634</v>
+      </c>
+      <c r="D78">
+        <v>8.7431103672622051E-2</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="2">
+        <f>AVERAGE(B71:I71)</f>
+        <v>4.9394200292716822E-2</v>
+      </c>
+      <c r="C82" s="2">
+        <f>_xlfn.STDEV.S(B71:I71)</f>
+        <v>7.4764027292336721E-2</v>
+      </c>
+      <c r="D82" s="2">
+        <f>MAX(B71:I71)</f>
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="2">
+        <f>AVERAGE(B72:I72)</f>
+        <v>0.1499615062542845</v>
+      </c>
+      <c r="C83" s="2">
+        <f>_xlfn.STDEV.S(B72:I72)</f>
+        <v>0.219338057045979</v>
+      </c>
+      <c r="D83" s="2">
+        <f>MAX(B72:I72)</f>
+        <v>0.64215249846663691</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="2">
+        <f>AVERAGE(B73:I73)</f>
+        <v>4.9394200292716822E-2</v>
+      </c>
+      <c r="C84" s="2">
+        <f>_xlfn.STDEV.S(B73:I73)</f>
+        <v>7.4764027292336721E-2</v>
+      </c>
+      <c r="D84" s="2">
+        <f>MAX(B73:I73)</f>
+        <v>0.19661138755800142</v>
+      </c>
+      <c r="E84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="2">
+        <f>AVERAGE(B74:I74)</f>
+        <v>8.1857991034877051E-2</v>
+      </c>
+      <c r="C85" s="2">
+        <f>_xlfn.STDEV.S(B74:I74)</f>
+        <v>0.11748009866307094</v>
+      </c>
+      <c r="D85" s="2">
+        <f>MAX(B74:I74)</f>
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="E85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="2">
+        <f>AVERAGE(B75:I75)</f>
+        <v>8.1857991034877051E-2</v>
+      </c>
+      <c r="C86" s="2">
+        <f>_xlfn.STDEV.S(B75:I75)</f>
+        <v>0.11748009866307094</v>
+      </c>
+      <c r="D86" s="2">
+        <f>MAX(B75:I75)</f>
+        <v>0.28055540199237605</v>
+      </c>
+      <c r="E86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="2">
+        <f>AVERAGE(B76:I76)</f>
+        <v>0.17665009931648273</v>
+      </c>
+      <c r="C87" s="2">
+        <f>_xlfn.STDEV.S(B76:I76)</f>
+        <v>0.22810216643738657</v>
+      </c>
+      <c r="D87" s="2">
+        <f>MAX(B76:I76)</f>
+        <v>0.64215249846663691</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="2">
+        <f>AVERAGE(B77:I77)</f>
+        <v>6.6294445280032213E-2</v>
+      </c>
+      <c r="C88" s="2">
+        <f>_xlfn.STDEV.S(B77:I77)</f>
+        <v>9.2773143145448794E-2</v>
+      </c>
+      <c r="D88" s="2">
+        <f>MAX(B77:I77)</f>
+        <v>0.20993749208047283</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>66</v>
+      </c>
+      <c r="B89" s="2">
+        <f>AVERAGE(B78:I78)</f>
+        <v>4.2397372974610062E-2</v>
+      </c>
+      <c r="C89" s="2">
+        <f>_xlfn.STDEV.S(B78:I78)</f>
+        <v>6.3141678471170845E-2</v>
+      </c>
+      <c r="D89" s="2">
+        <f>MAX(B78:I78)</f>
+        <v>0.16431677645163634</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>67</v>
+      </c>
+      <c r="B90" s="2">
+        <f>AVERAGE(B79:I79)</f>
+        <v>0</v>
+      </c>
+      <c r="C90" s="2">
+        <f>_xlfn.STDEV.S(B79:I79)</f>
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <f>MAX(B79:I79)</f>
+        <v>0</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5406,17 +5165,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27993049-2CCD-4834-B543-67CBD9F6FBE5}">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -5442,7 +5201,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -5454,40 +5213,40 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>95</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
         <v>96</v>
       </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>97</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>98</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>99</v>
       </c>
-      <c r="P1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>100</v>
-      </c>
-      <c r="R1" t="s">
-        <v>101</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -5495,7 +5254,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5516,7 +5275,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5534,7 +5293,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -5552,7 +5311,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -5570,7 +5329,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -5591,7 +5350,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5609,7 +5368,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -5624,7 +5383,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9">
         <f>COUNTIF(B2:B8,"&gt;0")</f>
@@ -5770,10 +5529,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -6163,7 +5922,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <f t="shared" ref="B18:R18" si="9">(B7/$S7)*B$10</f>
@@ -6240,7 +5999,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19">
         <f t="shared" ref="B19:R19" si="10">(B8/$S8)*B$10</f>
@@ -6317,7 +6076,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -6370,7 +6129,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <f t="shared" si="11"/>
@@ -6382,7 +6141,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <f t="shared" si="11"/>
@@ -6394,7 +6153,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -6433,9 +6192,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <f t="shared" si="12"/>
@@ -6445,9 +6204,9 @@
         <v>0.10116584392949407</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34">
         <f t="shared" si="12"/>
@@ -6457,27 +6216,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36" t="s">
-        <v>28</v>
-      </c>
-      <c r="O36" t="s">
-        <v>29</v>
-      </c>
-      <c r="P36" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>31</v>
-      </c>
-      <c r="R36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -6488,267 +6232,49 @@
       <c r="D37">
         <v>0.45323472054363229</v>
       </c>
-      <c r="H37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37">
-        <v>7.9399712977057516E-2</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0.29556045383134949</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37" s="2">
-        <f t="shared" ref="O37:O43" si="13">AVERAGE(I37:N37)</f>
-        <v>6.2493361134734499E-2</v>
-      </c>
-      <c r="P37" s="2">
-        <f t="shared" ref="P37:P43" si="14">_xlfn.STDEV.S(I37:N37)</f>
-        <v>0.11851394447433966</v>
-      </c>
-      <c r="Q37" s="2">
-        <f t="shared" ref="Q37:Q43" si="15">MAX(I37:N37)</f>
-        <v>0.29556045383134949</v>
-      </c>
-      <c r="R37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
       <c r="B38">
-        <f t="shared" ref="B38:B40" si="16">(SUMPRODUCT($B$15:$R$15,B17:R17)/($S$15*S17))</f>
+        <f t="shared" ref="B38:B40" si="13">(SUMPRODUCT($B$15:$R$15,B17:R17)/($S$15*S17))</f>
         <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="H38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38">
-        <v>7.9399712977057516E-2</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0.10116584392949407</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38" s="2">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
         <f t="shared" si="13"/>
-        <v>3.0094259484425262E-2</v>
-      </c>
-      <c r="P38" s="2">
-        <f t="shared" si="14"/>
-        <v>4.7127180427669023E-2</v>
-      </c>
-      <c r="Q38" s="2">
-        <f t="shared" si="15"/>
-        <v>0.10116584392949407</v>
-      </c>
-      <c r="R38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="H39" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0.45323472054363229</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39" s="2">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40">
         <f t="shared" si="13"/>
-        <v>7.5539120090605386E-2</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="14"/>
-        <v>0.1850322998408046</v>
-      </c>
-      <c r="Q39" s="2">
-        <f t="shared" si="15"/>
-        <v>0.45323472054363229</v>
-      </c>
-      <c r="R39" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0.45323472054363229</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40" s="2">
-        <f t="shared" si="13"/>
-        <v>7.5539120090605386E-2</v>
-      </c>
-      <c r="P40" s="2">
-        <f t="shared" si="14"/>
-        <v>0.1850322998408046</v>
-      </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="15"/>
-        <v>0.45323472054363229</v>
-      </c>
-      <c r="R40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41" s="2">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P41" s="2">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="Q41" s="2">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="H42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I42">
-        <v>0.29556045383134949</v>
-      </c>
-      <c r="J42">
-        <v>0.10116584392949407</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42" s="2">
-        <f t="shared" si="13"/>
-        <v>6.612104962680726E-2</v>
-      </c>
-      <c r="P42" s="2">
-        <f t="shared" si="14"/>
-        <v>0.11946426296131893</v>
-      </c>
-      <c r="Q42" s="2">
-        <f t="shared" si="15"/>
-        <v>0.29556045383134949</v>
-      </c>
-      <c r="R42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -6756,96 +6282,780 @@
         <f>(SUMPRODUCT($B$16:$R$16,B17:R17)/($S$16*S17))</f>
         <v>0</v>
       </c>
-      <c r="H43" t="s">
-        <v>66</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43" s="2">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="2">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ref="B44:B45" si="14">(SUMPRODUCT($B$16:$R$16,B18:R18)/($S$16*S18))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="2">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <f t="shared" ref="B44:B45" si="17">(SUMPRODUCT($B$16:$R$16,B18:R18)/($S$16*S18))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48">
         <f>(SUMPRODUCT($B$17:$R$17,B18:R18)/($S$17*S18))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49">
         <f>(SUMPRODUCT($B$17:$R$17,B19:R19)/($S$17*S19))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52">
         <f>(SUMPRODUCT($B$18:$R$18,B19:R19)/($S$18*S19))</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55">
+        <v>7.9399712977057516E-2</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0.29556045383134949</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>7.9399712977057516E-2</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0.10116584392949407</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0.45323472054363229</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.45323472054363229</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60">
+        <v>0.29556045383134949</v>
+      </c>
+      <c r="C60">
+        <v>0.10116584392949407</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="2">
+        <f>AVERAGE(B55:G55)</f>
+        <v>6.2493361134734499E-2</v>
+      </c>
+      <c r="C64" s="2">
+        <f>_xlfn.STDEV.S(B55:G55)</f>
+        <v>0.11851394447433966</v>
+      </c>
+      <c r="D64" s="2">
+        <f>MAX(B55:G55)</f>
+        <v>0.29556045383134949</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="2">
+        <f>AVERAGE(B56:G56)</f>
+        <v>3.0094259484425262E-2</v>
+      </c>
+      <c r="C65" s="2">
+        <f>_xlfn.STDEV.S(B56:G56)</f>
+        <v>4.7127180427669023E-2</v>
+      </c>
+      <c r="D65" s="2">
+        <f>MAX(B56:G56)</f>
+        <v>0.10116584392949407</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="2">
+        <f>AVERAGE(B57:G57)</f>
+        <v>7.5539120090605386E-2</v>
+      </c>
+      <c r="C66" s="2">
+        <f>_xlfn.STDEV.S(B57:G57)</f>
+        <v>0.1850322998408046</v>
+      </c>
+      <c r="D66" s="2">
+        <f>MAX(B57:G57)</f>
+        <v>0.45323472054363229</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="2">
+        <f>AVERAGE(B58:G58)</f>
+        <v>7.5539120090605386E-2</v>
+      </c>
+      <c r="C67" s="2">
+        <f>_xlfn.STDEV.S(B58:G58)</f>
+        <v>0.1850322998408046</v>
+      </c>
+      <c r="D67" s="2">
+        <f>MAX(B58:G58)</f>
+        <v>0.45323472054363229</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="2">
+        <f>AVERAGE(B59:G59)</f>
+        <v>0</v>
+      </c>
+      <c r="C68" s="2">
+        <f>_xlfn.STDEV.S(B59:G59)</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="2">
+        <f>MAX(B59:G59)</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" s="2">
+        <f>AVERAGE(B60:G60)</f>
+        <v>6.612104962680726E-2</v>
+      </c>
+      <c r="C69" s="2">
+        <f>_xlfn.STDEV.S(B60:G60)</f>
+        <v>0.11946426296131893</v>
+      </c>
+      <c r="D69" s="2">
+        <f>MAX(B60:G60)</f>
+        <v>0.29556045383134949</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="2">
+        <f>AVERAGE(B61:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="C70" s="2">
+        <f>_xlfn.STDEV.S(B61:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="D70" s="2">
+        <f>MAX(B61:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28894055-7F27-471F-8199-8B27A85BFA58}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>